<commit_message>
Add Auto Cal, Fix bugs
</commit_message>
<xml_diff>
--- a/documents/pinout.xlsx
+++ b/documents/pinout.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-560" yWindow="0" windowWidth="51200" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="-555" yWindow="0" windowWidth="43440" windowHeight="18240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pinout" sheetId="1" r:id="rId1"/>
-    <sheet name="Questions" sheetId="2" r:id="rId2"/>
-    <sheet name="Range Selection" sheetId="3" r:id="rId3"/>
-    <sheet name="asm Sampling Routine" sheetId="4" r:id="rId4"/>
-    <sheet name="features" sheetId="5" r:id="rId5"/>
+    <sheet name="Range Selection" sheetId="3" r:id="rId2"/>
+    <sheet name="asm Sampling Routine" sheetId="4" r:id="rId3"/>
+    <sheet name="features" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="calval0v1">'Range Selection'!$C$59</definedName>
+    <definedName name="calval3v3">'Range Selection'!$C$45</definedName>
+  </definedNames>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="263">
   <si>
     <t>DSO-138</t>
   </si>
@@ -331,12 +334,6 @@
     <t>Voltage Generation</t>
   </si>
   <si>
-    <t>VSENSEL1/VSENSEL2/CPLSEL</t>
-  </si>
-  <si>
-    <t>V-MON/VGEN</t>
-  </si>
-  <si>
     <t>AMPSEL</t>
   </si>
   <si>
@@ -403,12 +400,6 @@
     <t>Y/N</t>
   </si>
   <si>
-    <t>Dual Button/Display Use</t>
-  </si>
-  <si>
-    <t>Questions</t>
-  </si>
-  <si>
     <t>Sel0</t>
   </si>
   <si>
@@ -469,12 +460,6 @@
     <t>Connector</t>
   </si>
   <si>
-    <t>How does this work on DSO-138?</t>
-  </si>
-  <si>
-    <t>How does this work on DSO-150?</t>
-  </si>
-  <si>
     <t>if DELAY &lt; 0</t>
   </si>
   <si>
@@ -818,6 +803,18 @@
   </si>
   <si>
     <t>Coupling Mode (AC/DC/GND)</t>
+  </si>
+  <si>
+    <t>3.3V Cal</t>
+  </si>
+  <si>
+    <t>0.1V Cal</t>
+  </si>
+  <si>
+    <t>Calval</t>
+  </si>
+  <si>
+    <t>calval</t>
   </si>
 </sst>
 </file>
@@ -878,7 +875,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -898,6 +895,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -962,13 +965,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1024,7 +1028,653 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3.3V</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$A$46:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$B$46:$B$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>865</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1704</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2218</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2213</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0.1V</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$A$60:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$B$60:$B$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>744</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1490</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2174</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="176454272"/>
+        <c:axId val="176456064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="176454272"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176456064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="176456064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176454272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.2812148481439817E-2"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.75457513756726358"/>
+          <c:h val="0.8326195683872849"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>3.3V</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$A$46:$A$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$F$46:$F$57</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>9.7058823529411753E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8507462686567154E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7633136094674548E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8214285714285712E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8507462686567154E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9075144508670518E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.936619718309859E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.9756537421100088E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4559421599638492E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30358785648574055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0.1V</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$A$60:$A$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Range Selection'!$F$60:$F$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>7.3880597014925357E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3880597014925357E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.8507462686567137E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2350746268656699E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2350746268656699E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8507462686567137E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.983864461476399E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.983864461476399E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9502487562189035E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9301877708233011E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9168586597215246E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3593486111301815E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="176485120"/>
+        <c:axId val="176486656"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="176485120"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176486656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="176486656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="176485120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1351,20 +2001,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.1640625" customWidth="1"/>
-    <col min="3" max="4" width="23.1640625" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="4" width="23.125" customWidth="1"/>
+    <col min="5" max="5" width="43.625" customWidth="1"/>
     <col min="6" max="6" width="5.5" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" customWidth="1"/>
+    <col min="7" max="7" width="36.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1382,10 +2032,10 @@
         <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1405,7 +2055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1416,16 +2066,16 @@
         <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1436,16 +2086,16 @@
         <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
         <v>98</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1453,19 +2103,19 @@
         <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
         <v>97</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1476,16 +2126,16 @@
         <v>89</v>
       </c>
       <c r="D8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E8" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1499,13 +2149,13 @@
         <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1522,10 +2172,10 @@
         <v>79</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1539,16 +2189,16 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +2218,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1588,10 +2238,10 @@
         <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1611,10 +2261,10 @@
         <v>41</v>
       </c>
       <c r="G14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1634,10 +2284,10 @@
         <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1657,10 +2307,10 @@
         <v>41</v>
       </c>
       <c r="G16" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1680,10 +2330,10 @@
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1703,10 +2353,10 @@
         <v>41</v>
       </c>
       <c r="G18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1720,16 +2370,16 @@
         <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>41</v>
       </c>
       <c r="G19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1743,13 +2393,13 @@
         <v>57</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1763,13 +2413,13 @@
         <v>58</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1786,10 +2436,10 @@
         <v>77</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1803,13 +2453,13 @@
         <v>60</v>
       </c>
       <c r="E24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1823,13 +2473,13 @@
         <v>61</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1843,13 +2493,13 @@
         <v>62</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1863,13 +2513,13 @@
         <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1883,13 +2533,13 @@
         <v>64</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1903,13 +2553,13 @@
         <v>65</v>
       </c>
       <c r="E29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1926,10 +2576,10 @@
         <v>80</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1940,16 +2590,16 @@
         <v>79</v>
       </c>
       <c r="D31" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" t="s">
         <v>112</v>
       </c>
-      <c r="E31" t="s">
-        <v>114</v>
-      </c>
       <c r="F31" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1960,16 +2610,16 @@
         <v>80</v>
       </c>
       <c r="D32" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1980,19 +2630,19 @@
         <v>81</v>
       </c>
       <c r="D33" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2006,13 +2656,13 @@
         <v>33</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G34" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2026,13 +2676,13 @@
         <v>34</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2046,13 +2696,13 @@
         <v>35</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G36" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2072,7 +2722,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2092,7 +2742,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2125,54 +2775,1320 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B6"/>
+  <dimension ref="A2:G71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
+    <col min="7" max="7" width="15.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B17" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B18" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>224</v>
+      </c>
+      <c r="B19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>229</v>
+      </c>
+      <c r="B25" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>230</v>
+      </c>
+      <c r="B26" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>232</v>
+      </c>
+      <c r="B28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>233</v>
+      </c>
+      <c r="B29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>259</v>
+      </c>
+      <c r="B45" t="s">
+        <v>261</v>
+      </c>
+      <c r="C45">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>17</v>
+      </c>
+      <c r="D46">
+        <f>1/A46</f>
+        <v>0.05</v>
+      </c>
+      <c r="E46">
+        <f>B46/D46</f>
+        <v>340</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" ref="F46:F57" si="0">calval3v3/E46</f>
+        <v>9.7058823529411753E-3</v>
+      </c>
+      <c r="G46">
+        <f>calval3v3/B46</f>
+        <v>0.19411764705882351</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <f>B47/B46</f>
+        <v>1.9411764705882353</v>
+      </c>
+      <c r="D47">
+        <f>1/A47</f>
+        <v>0.1</v>
+      </c>
+      <c r="E47">
+        <f t="shared" ref="E47:E57" si="1">B47/D47</f>
+        <v>330</v>
+      </c>
+      <c r="F47" s="6">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="G47">
+        <f>calval3v3/B47</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>67</v>
+      </c>
+      <c r="C48">
+        <f t="shared" ref="C48:C57" si="2">B48/B47</f>
+        <v>2.0303030303030303</v>
+      </c>
+      <c r="D48">
+        <f>1/A48</f>
+        <v>0.2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>335</v>
+      </c>
+      <c r="F48" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8507462686567154E-3</v>
+      </c>
+      <c r="G48">
+        <f>calval3v3/B48</f>
+        <v>4.9253731343283577E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>169</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>2.5223880597014925</v>
+      </c>
+      <c r="D49">
+        <v>0.5</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>338</v>
+      </c>
+      <c r="F49" s="6">
+        <f t="shared" si="0"/>
+        <v>9.7633136094674548E-3</v>
+      </c>
+      <c r="G49">
+        <f>calval3v3/B49</f>
+        <v>1.952662721893491E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>336</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>1.9881656804733727</v>
+      </c>
+      <c r="D50">
+        <f>1/A50</f>
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>336</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8214285714285712E-3</v>
+      </c>
+      <c r="G50">
+        <f>calval3v3/B50</f>
+        <v>9.8214285714285712E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>0.5</v>
+      </c>
+      <c r="B51">
+        <v>670</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>1.9940476190476191</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ref="D51:D57" si="3">1/A51</f>
+        <v>2</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>335</v>
+      </c>
+      <c r="F51" s="6">
+        <f t="shared" si="0"/>
+        <v>9.8507462686567154E-3</v>
+      </c>
+      <c r="G51">
+        <f>calval3v3/B51</f>
+        <v>4.9253731343283577E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>0.2</v>
+      </c>
+      <c r="B52">
+        <v>865</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>1.291044776119403</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>173</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>1.9075144508670518E-2</v>
+      </c>
+      <c r="G52">
+        <f>calval3v3/B52</f>
+        <v>3.8150289017341039E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>0.1</v>
+      </c>
+      <c r="B53">
+        <v>1704</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>1.9699421965317918</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>170.4</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>1.936619718309859E-2</v>
+      </c>
+      <c r="G53">
+        <f>calval3v3/B53</f>
+        <v>1.936619718309859E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>0.05</v>
+      </c>
+      <c r="B54">
+        <v>2218</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>1.301643192488263</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>110.9</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>2.9756537421100088E-2</v>
+      </c>
+      <c r="G54">
+        <f>calval3v3/B54</f>
+        <v>1.4878268710550044E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>0.02</v>
+      </c>
+      <c r="B55">
+        <v>2213</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>0.99774571686203783</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>44.26</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>7.4559421599638492E-2</v>
+      </c>
+      <c r="G55">
+        <f>calval3v3/B55</f>
+        <v>1.49118843199277E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>0.01</v>
+      </c>
+      <c r="B56">
+        <v>2200</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>0.99412562132851334</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="G56">
+        <f>calval3v3/B56</f>
+        <v>1.4999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B57">
+        <v>2174</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="2"/>
+        <v>0.98818181818181816</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>10.87</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>0.30358785648574055</v>
+      </c>
+      <c r="G57">
+        <f>calval3v3/B57</f>
+        <v>1.5179392824287029E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>260</v>
+      </c>
+      <c r="B59" t="s">
+        <v>262</v>
+      </c>
+      <c r="C59">
+        <f>B65/B51*calval3v3</f>
+        <v>0.14776119402985072</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <f>1/A60</f>
+        <v>0.05</v>
+      </c>
+      <c r="E60">
+        <f>B60/D60</f>
+        <v>20</v>
+      </c>
+      <c r="F60">
+        <f t="shared" ref="F60:F71" si="4">calval0v1/E60</f>
+        <v>7.3880597014925357E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <f>B61/B60</f>
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ref="D61:D71" si="5">1/A61</f>
+        <v>0.1</v>
+      </c>
+      <c r="E61">
+        <f t="shared" ref="E61:E71" si="6">B61/D61</f>
+        <v>20</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="4"/>
+        <v>7.3880597014925357E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="C62">
+        <f t="shared" ref="C62:C71" si="7">B62/B61</f>
+        <v>1.5</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="5"/>
+        <v>0.2</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="4"/>
+        <v>9.8507462686567137E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="7"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="4"/>
+        <v>9.2350746268656699E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>16</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="4"/>
+        <v>9.2350746268656699E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>0.5</v>
+      </c>
+      <c r="B65">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="7"/>
+        <v>1.875</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="F65" s="6">
+        <f t="shared" si="4"/>
+        <v>9.8507462686567137E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>0.2</v>
+      </c>
+      <c r="B66">
+        <v>74</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="7"/>
+        <v>2.4666666666666668</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="6"/>
+        <v>14.8</v>
+      </c>
+      <c r="F66" s="6">
+        <f t="shared" si="4"/>
+        <v>9.983864461476399E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>0.1</v>
+      </c>
+      <c r="B67">
+        <v>148</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="6"/>
+        <v>14.8</v>
+      </c>
+      <c r="F67" s="6">
+        <f t="shared" si="4"/>
+        <v>9.983864461476399E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>0.05</v>
+      </c>
+      <c r="B68">
+        <v>297</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="7"/>
+        <v>2.0067567567567566</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="6"/>
+        <v>14.85</v>
+      </c>
+      <c r="F68" s="6">
+        <f t="shared" si="4"/>
+        <v>9.9502487562189035E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>0.02</v>
+      </c>
+      <c r="B69">
+        <v>744</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="7"/>
+        <v>2.5050505050505052</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>14.88</v>
+      </c>
+      <c r="F69" s="6">
+        <f t="shared" si="4"/>
+        <v>9.9301877708233011E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>0.01</v>
+      </c>
+      <c r="B70">
+        <v>1490</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="7"/>
+        <v>2.002688172043011</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>14.9</v>
+      </c>
+      <c r="F70" s="6">
+        <f t="shared" si="4"/>
+        <v>9.9168586597215246E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B71">
+        <v>2174</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="7"/>
+        <v>1.4590604026845637</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>200</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>10.87</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="4"/>
+        <v>1.3593486111301815E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E78"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="E23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C29" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>163</v>
+      </c>
+      <c r="C32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>154</v>
+      </c>
+      <c r="C34" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" t="s">
+        <v>169</v>
+      </c>
+      <c r="E35" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>163</v>
+      </c>
+      <c r="C36" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>172</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>175</v>
+      </c>
+      <c r="C39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>180</v>
+      </c>
+      <c r="C41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" t="s">
+        <v>199</v>
+      </c>
+      <c r="E44" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>163</v>
+      </c>
+      <c r="C48" t="s">
+        <v>204</v>
+      </c>
+      <c r="E48" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
         <v>149</v>
+      </c>
+      <c r="C49" t="s">
+        <v>206</v>
+      </c>
+      <c r="E49" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" t="s">
+        <v>209</v>
+      </c>
+      <c r="E52" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>175</v>
+      </c>
+      <c r="C53" t="s">
+        <v>211</v>
+      </c>
+      <c r="E53" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>213</v>
+      </c>
+      <c r="C54" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>216</v>
+      </c>
+      <c r="C57" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2186,696 +4102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F41"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>141</v>
-      </c>
-      <c r="F12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C13" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" t="s">
-        <v>141</v>
-      </c>
-      <c r="C14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D14" t="s">
-        <v>141</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>227</v>
-      </c>
-      <c r="B17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>229</v>
-      </c>
-      <c r="B18" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>230</v>
-      </c>
-      <c r="B19" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>231</v>
-      </c>
-      <c r="B20" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>228</v>
-      </c>
-      <c r="B21" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>232</v>
-      </c>
-      <c r="B22" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>233</v>
-      </c>
-      <c r="B23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>234</v>
-      </c>
-      <c r="B24" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>235</v>
-      </c>
-      <c r="B25" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>237</v>
-      </c>
-      <c r="B27" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>238</v>
-      </c>
-      <c r="B28" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>239</v>
-      </c>
-      <c r="B29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>251</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E78"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="B23" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" t="s">
-        <v>163</v>
-      </c>
-      <c r="E23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="B25" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" t="s">
-        <v>156</v>
-      </c>
-      <c r="E25" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="B26" t="s">
-        <v>158</v>
-      </c>
-      <c r="C26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" t="s">
-        <v>160</v>
-      </c>
-      <c r="C28" t="s">
-        <v>161</v>
-      </c>
-      <c r="E28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" t="s">
-        <v>167</v>
-      </c>
-      <c r="E29" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" t="s">
-        <v>169</v>
-      </c>
-      <c r="C30" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" t="s">
-        <v>160</v>
-      </c>
-      <c r="C31" t="s">
-        <v>171</v>
-      </c>
-      <c r="E31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C32" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="B34" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" t="s">
-        <v>173</v>
-      </c>
-      <c r="E34" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="B35" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="B36" t="s">
-        <v>169</v>
-      </c>
-      <c r="C36" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="B38" t="s">
-        <v>178</v>
-      </c>
-      <c r="C38" t="s">
-        <v>179</v>
-      </c>
-      <c r="E38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="B39" t="s">
-        <v>181</v>
-      </c>
-      <c r="C39" t="s">
-        <v>182</v>
-      </c>
-      <c r="E39" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="B40" t="s">
-        <v>184</v>
-      </c>
-      <c r="C40" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="B41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C41" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="B43" t="s">
-        <v>203</v>
-      </c>
-      <c r="C43" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="B44" t="s">
-        <v>204</v>
-      </c>
-      <c r="C44" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="B45" t="s">
-        <v>208</v>
-      </c>
-      <c r="C45" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="B48" t="s">
-        <v>169</v>
-      </c>
-      <c r="C48" t="s">
-        <v>210</v>
-      </c>
-      <c r="E48" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="B49" t="s">
-        <v>155</v>
-      </c>
-      <c r="C49" t="s">
-        <v>212</v>
-      </c>
-      <c r="E49" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="B50" t="s">
-        <v>158</v>
-      </c>
-      <c r="C50" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="B52" t="s">
-        <v>178</v>
-      </c>
-      <c r="C52" t="s">
-        <v>215</v>
-      </c>
-      <c r="E52" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="B53" t="s">
-        <v>181</v>
-      </c>
-      <c r="C53" t="s">
-        <v>217</v>
-      </c>
-      <c r="E53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="B54" t="s">
-        <v>219</v>
-      </c>
-      <c r="C54" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="B57" t="s">
-        <v>222</v>
-      </c>
-      <c r="C57" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>152</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A17"/>
   <sheetViews>
@@ -2883,84 +4110,84 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>